<commit_message>
Atribuição de tarefas task5
</commit_message>
<xml_diff>
--- a/Planilha_organização_tarefas.xlsx
+++ b/Planilha_organização_tarefas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andresa Marçal\Desktop\spring\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37612d9d55d913cf/Desktop/projeto_integradorOficial/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5726C11-F94F-4AFF-818C-7F29420C81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{F5726C11-F94F-4AFF-818C-7F29420C81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE1AC0F5-8F80-4340-86A8-7AA15545DD96}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bloco 02" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>DISTRIBUIÇÃO DAS TAREFAS – PROJETO INTEGRADOR</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Giselle de Souza Gabriel</t>
+  </si>
+  <si>
+    <t>João Vitor</t>
   </si>
 </sst>
 </file>
@@ -359,13 +362,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,9 +386,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2582,8 +2585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2600,13 +2603,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2615,11 +2618,11 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2641,18 +2644,18 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="21">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="22"/>
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="22"/>
+      <c r="G5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:26" ht="21">
       <c r="A6" s="6" t="s">
@@ -2675,16 +2678,16 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="12" t="s">
         <v>28</v>
       </c>
       <c r="I7" s="8"/>
@@ -2707,14 +2710,14 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -2735,14 +2738,14 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -2763,14 +2766,14 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -2791,142 +2794,142 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="12"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14" t="s">
+      <c r="G11" s="15"/>
+      <c r="H11" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:26" ht="20.399999999999999">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="20.399999999999999">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="22" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20.399999999999999">
-      <c r="A17" s="16"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="16"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="20.399999999999999">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="16"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.399999999999999">
-      <c r="A19" s="17"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="17"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="10"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="14"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="14" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="12"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="14" t="s">
+      <c r="G20" s="15"/>
+      <c r="H20" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
@@ -2934,18 +2937,18 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="D25" s="20" t="s">
+      <c r="B25" s="22"/>
+      <c r="D25" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="G25" s="20" t="s">
+      <c r="E25" s="22"/>
+      <c r="G25" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="21"/>
+      <c r="H25" s="22"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -2968,160 +2971,164 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="14" t="s">
-        <v>11</v>
+      <c r="A27" s="15"/>
+      <c r="B27" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="14"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" ht="36" customHeight="1">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="14"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="14"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="14"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="12"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A35" s="15"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D35" s="15"/>
+      <c r="D35" s="16"/>
       <c r="E35" s="9"/>
-      <c r="G35" s="15"/>
+      <c r="G35" s="16"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="9"/>
-      <c r="G36" s="16"/>
+      <c r="G36" s="17"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A37" s="16"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
-      <c r="D37" s="16"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="16"/>
+      <c r="G37" s="17"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A38" s="16"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="9" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="9"/>
-      <c r="G38" s="16"/>
+      <c r="G38" s="17"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A39" s="17"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="10"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A40" s="11"/>
-      <c r="B40" s="14"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="14"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="14"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="12"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
       <c r="B44" s="4"/>
@@ -7910,35 +7917,9 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="D35:D39"/>
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="E27:E30"/>
     <mergeCell ref="H27:H30"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="E31:E34"/>
@@ -7955,10 +7936,36 @@
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="D31:D34"/>
     <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="G40:G43"/>
     <mergeCell ref="G31:G34"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="E27:E30"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
@@ -7987,24 +7994,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
@@ -8024,18 +8031,18 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="21">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="22"/>
+      <c r="D5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="G5" s="20" t="s">
+      <c r="E5" s="22"/>
+      <c r="G5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:26" ht="21">
       <c r="A6" s="6" t="s">
@@ -8058,14 +8065,14 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="12"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -8086,14 +8093,14 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -8114,14 +8121,14 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -8142,14 +8149,14 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -8170,118 +8177,118 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="12"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="12"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:26" ht="20.399999999999999">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="9"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:26" ht="20.399999999999999">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="9"/>
-      <c r="G16" s="16"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" ht="20.399999999999999">
-      <c r="A17" s="16"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="9"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="20.399999999999999">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="9"/>
-      <c r="G18" s="16"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="20.399999999999999">
-      <c r="A19" s="17"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="17"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="10"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="14"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="14"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="12"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="12"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
@@ -8289,18 +8296,18 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="D25" s="20" t="s">
+      <c r="B25" s="22"/>
+      <c r="D25" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="G25" s="20" t="s">
+      <c r="E25" s="22"/>
+      <c r="G25" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="21"/>
+      <c r="H25" s="22"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -8323,158 +8330,158 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="14"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" ht="33" customHeight="1">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="14"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="14"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="14"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="12"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="12"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A35" s="15"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="15"/>
+      <c r="D35" s="16"/>
       <c r="E35" s="9"/>
-      <c r="G35" s="15"/>
+      <c r="G35" s="16"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="9"/>
-      <c r="G36" s="16"/>
+      <c r="G36" s="17"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A37" s="16"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="16"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="16"/>
+      <c r="G37" s="17"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A38" s="16"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="9"/>
-      <c r="G38" s="16"/>
+      <c r="G38" s="17"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A39" s="17"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="10"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A40" s="11"/>
-      <c r="B40" s="14"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="14"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="14"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="12"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="12"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
       <c r="B44" s="4"/>
@@ -8482,14 +8489,14 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="D45" s="20" t="s">
+      <c r="B45" s="22"/>
+      <c r="D45" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="21"/>
+      <c r="E45" s="22"/>
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1">
@@ -8508,136 +8515,136 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A47" s="11"/>
-      <c r="B47" s="14"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="14"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="12"/>
       <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
       <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A51" s="11"/>
-      <c r="B51" s="14"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="14"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="12"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="12"/>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A55" s="15"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="15"/>
+      <c r="D55" s="16"/>
       <c r="E55" s="9"/>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A56" s="16"/>
+      <c r="A56" s="17"/>
       <c r="B56" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="16"/>
+      <c r="D56" s="17"/>
       <c r="E56" s="9"/>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A57" s="16"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="16"/>
+      <c r="D57" s="17"/>
       <c r="E57" s="9"/>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A58" s="16"/>
+      <c r="A58" s="17"/>
       <c r="B58" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="16"/>
+      <c r="D58" s="17"/>
       <c r="E58" s="9"/>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A59" s="17"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="17"/>
+      <c r="D59" s="18"/>
       <c r="E59" s="10"/>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A60" s="11"/>
-      <c r="B60" s="14"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="14"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="12"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="12"/>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1">
@@ -13327,40 +13334,21 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="D55:D59"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="E27:E30"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="G15:G19"/>
@@ -13377,21 +13365,40 @@
     <mergeCell ref="H27:H30"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="E31:E34"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="D35:D39"/>
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="D55:D59"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>

</xml_diff>

<commit_message>
Destribuição de tarefas task 6
</commit_message>
<xml_diff>
--- a/Planilha_organização_tarefas.xlsx
+++ b/Planilha_organização_tarefas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37612d9d55d913cf/Desktop/projeto_integradorOficial/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{F5726C11-F94F-4AFF-818C-7F29420C81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE1AC0F5-8F80-4340-86A8-7AA15545DD96}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E24E055-19C9-4C32-96BF-81CCF229DE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,19 @@
     <sheet name="Bloco 02" sheetId="1" r:id="rId1"/>
     <sheet name="Bloco 03" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mh5Ks4+mtfOQnaXufRUTzqKSoieFg=="/>
     </ext>
@@ -26,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
   <si>
     <t>DISTRIBUIÇÃO DAS TAREFAS – PROJETO INTEGRADOR</t>
   </si>
@@ -58,8 +69,14 @@
     <t>João Vitor Moreira</t>
   </si>
   <si>
+    <t>Daisy Viana</t>
+  </si>
+  <si>
     <t xml:space="preserve">Giselle de Souza Gabriel
 </t>
+  </si>
+  <si>
+    <t>Andresa Marçal</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -71,6 +88,9 @@
   <si>
     <t xml:space="preserve">Daisy Kelly Viana 
 </t>
+  </si>
+  <si>
+    <t>Giselle de Souza Gabriel</t>
   </si>
   <si>
     <t xml:space="preserve">Nicolle Sanches
@@ -92,6 +112,15 @@
   </si>
   <si>
     <t>TASK 07</t>
+  </si>
+  <si>
+    <t>João Vitor</t>
+  </si>
+  <si>
+    <t>Andressa Camillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yngrid Padilha </t>
   </si>
   <si>
     <t>TASK 08</t>
@@ -117,24 +146,12 @@
   <si>
     <t>TASK 15</t>
   </si>
-  <si>
-    <t>Daisy Viana</t>
-  </si>
-  <si>
-    <t>Andresa Marçal</t>
-  </si>
-  <si>
-    <t>Giselle de Souza Gabriel</t>
-  </si>
-  <si>
-    <t>João Vitor</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +194,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -334,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,24 +391,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2585,31 +2612,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="46.109375" customWidth="1"/>
-    <col min="6" max="6" width="2.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="46.109375" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="46.140625" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2618,11 +2645,11 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2630,7 +2657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26" ht="14.45">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -2638,24 +2665,24 @@
       <c r="F3" s="5"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="14.4">
+    <row r="4" spans="1:26" ht="14.45">
       <c r="B4" s="4"/>
       <c r="E4" s="4"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="21">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="D5" s="21" t="s">
+      <c r="B5" s="20"/>
+      <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="20"/>
+      <c r="G5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:26" ht="21">
       <c r="A6" s="6" t="s">
@@ -2678,17 +2705,17 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A7" s="15"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="15"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="12" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -2710,14 +2737,14 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -2738,14 +2765,14 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -2766,14 +2793,14 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -2794,142 +2821,142 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A11" s="15"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="12"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:26" ht="20.399999999999999">
-      <c r="A15" s="16"/>
-      <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="9" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="20.399999999999999">
-      <c r="A16" s="17"/>
-      <c r="B16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="9" t="s">
+    </row>
+    <row r="12" spans="1:26" ht="20.25" customHeight="1">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:26" ht="20.25" customHeight="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:26" ht="20.25" customHeight="1">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:26" ht="20.45">
+      <c r="A15" s="14"/>
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="20.399999999999999">
-      <c r="A17" s="17"/>
-      <c r="B17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="9" t="s">
+      <c r="D15" s="14"/>
+      <c r="E15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="9" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.399999999999999">
-      <c r="A18" s="17"/>
-      <c r="B18" s="9" t="s">
-        <v>11</v>
+    <row r="16" spans="1:26" ht="20.45">
+      <c r="A16" s="23"/>
+      <c r="B16" s="9" t="s">
+        <v>13</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="9" t="s">
+      <c r="D16" s="23"/>
+      <c r="E16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="20.399999999999999">
-      <c r="A19" s="18"/>
-      <c r="B19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="10"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="12"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="12" t="s">
+      <c r="G16" s="23"/>
+      <c r="H16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="20.45">
+      <c r="A17" s="23"/>
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="20.45">
+      <c r="A18" s="23"/>
+      <c r="B18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20.45">
+      <c r="A19" s="24"/>
+      <c r="B19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="10"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="13"/>
       <c r="H20" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
@@ -2937,18 +2964,18 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="21" t="s">
-        <v>17</v>
+      <c r="A25" s="16" t="s">
+        <v>20</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="D25" s="21" t="s">
-        <v>18</v>
+      <c r="B25" s="20"/>
+      <c r="D25" s="16" t="s">
+        <v>21</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="G25" s="21" t="s">
-        <v>19</v>
+      <c r="E25" s="20"/>
+      <c r="G25" s="16" t="s">
+        <v>22</v>
       </c>
-      <c r="H25" s="22"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -2971,164 +2998,177 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="12" t="s">
-        <v>12</v>
+      <c r="A27" s="13"/>
+      <c r="B27" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="12"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="15"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" ht="36" customHeight="1">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A31" s="15"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A35" s="14"/>
+      <c r="B35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="12"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A35" s="16"/>
-      <c r="B35" s="9" t="s">
+      <c r="D35" s="14"/>
+      <c r="E35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A36" s="23"/>
+      <c r="B36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="23"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A37" s="23"/>
+      <c r="B37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="23"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A38" s="23"/>
+      <c r="B38" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="23"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A39" s="24"/>
+      <c r="B39" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="9"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="17"/>
-      <c r="B36" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="9"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A37" s="17"/>
-      <c r="B37" s="9" t="s">
+      <c r="D39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A40" s="13"/>
+      <c r="B40" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="9"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A38" s="17"/>
-      <c r="B38" s="9" t="s">
-        <v>31</v>
+      <c r="D40" s="13"/>
+      <c r="E40" s="17" t="s">
+        <v>25</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="9"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A39" s="18"/>
-      <c r="B39" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="10"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="10"/>
-    </row>
-    <row r="40" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A40" s="15"/>
-      <c r="B40" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="12"/>
-      <c r="G40" s="15"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
     </row>
     <row r="42" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
     </row>
     <row r="43" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
       <c r="B44" s="4"/>
@@ -7917,25 +7957,24 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="G15:G19"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="E27:E30"/>
     <mergeCell ref="H27:H30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="G15:G19"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="H20:H23"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D31:D34"/>
     <mergeCell ref="G27:G30"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="G20:G23"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D5:E5"/>
@@ -7944,17 +7983,14 @@
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="A7:A10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="G7:G10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="D15:D19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="G20:G23"/>
     <mergeCell ref="H40:H43"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A35:A39"/>
@@ -7966,6 +8002,10 @@
     <mergeCell ref="E40:E43"/>
     <mergeCell ref="G40:G43"/>
     <mergeCell ref="G31:G34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="D31:D34"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
@@ -7980,44 +8020,44 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="46.109375" customWidth="1"/>
-    <col min="6" max="6" width="2.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="46.109375" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="46.140625" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26" ht="14.45">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -8025,24 +8065,24 @@
       <c r="F3" s="5"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="14.4">
+    <row r="4" spans="1:26" ht="14.45">
       <c r="B4" s="4"/>
       <c r="E4" s="4"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="21">
-      <c r="A5" s="21" t="s">
-        <v>20</v>
+      <c r="A5" s="16" t="s">
+        <v>26</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="D5" s="21" t="s">
-        <v>21</v>
+      <c r="B5" s="20"/>
+      <c r="D5" s="16" t="s">
+        <v>27</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="G5" s="21" t="s">
-        <v>22</v>
+      <c r="E5" s="20"/>
+      <c r="G5" s="16" t="s">
+        <v>28</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:26" ht="21">
       <c r="A6" s="6" t="s">
@@ -8065,13 +8105,13 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A7" s="15"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="12"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="15"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="12"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="12"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -8093,14 +8133,14 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -8121,14 +8161,14 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -8149,14 +8189,14 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -8177,118 +8217,118 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A11" s="15"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="12"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="12"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:26" ht="20.399999999999999">
-      <c r="A15" s="16"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:26" ht="20.45">
+      <c r="A15" s="14"/>
       <c r="B15" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="9"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:26" ht="20.399999999999999">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:26" ht="20.45">
+      <c r="A16" s="23"/>
       <c r="B16" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D16" s="17"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="9"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="20.399999999999999">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:8" ht="20.45">
+      <c r="A17" s="23"/>
       <c r="B17" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D17" s="17"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="9"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="20.399999999999999">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:8" ht="20.45">
+      <c r="A18" s="23"/>
       <c r="B18" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D18" s="17"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="9"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="20.399999999999999">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:8" ht="20.45">
+      <c r="A19" s="24"/>
       <c r="B19" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="10"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A20" s="15"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="12"/>
-      <c r="D20" s="15"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="12"/>
-      <c r="G20" s="15"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
@@ -8296,18 +8336,18 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="21" t="s">
-        <v>23</v>
+      <c r="A25" s="16" t="s">
+        <v>29</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="D25" s="21" t="s">
-        <v>24</v>
+      <c r="B25" s="20"/>
+      <c r="D25" s="16" t="s">
+        <v>30</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="G25" s="21" t="s">
-        <v>25</v>
+      <c r="E25" s="20"/>
+      <c r="G25" s="16" t="s">
+        <v>31</v>
       </c>
-      <c r="H25" s="22"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -8330,158 +8370,158 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="15"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="12"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="15"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="12"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="15"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" ht="33" customHeight="1">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A31" s="15"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="12"/>
-      <c r="D31" s="15"/>
+      <c r="D31" s="13"/>
       <c r="E31" s="12"/>
-      <c r="G31" s="15"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A35" s="16"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D35" s="16"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="9"/>
-      <c r="G35" s="16"/>
+      <c r="G35" s="14"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="17"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D36" s="17"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="9"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A37" s="17"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D37" s="17"/>
+      <c r="D37" s="23"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="23"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A38" s="17"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D38" s="17"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="9"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="23"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A39" s="18"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D39" s="18"/>
+      <c r="D39" s="24"/>
       <c r="E39" s="10"/>
-      <c r="G39" s="18"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A40" s="15"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="12"/>
-      <c r="D40" s="15"/>
+      <c r="D40" s="13"/>
       <c r="E40" s="12"/>
-      <c r="G40" s="15"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
     </row>
     <row r="42" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
     </row>
     <row r="43" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
       <c r="B44" s="4"/>
@@ -8489,14 +8529,14 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A45" s="21" t="s">
-        <v>26</v>
+      <c r="A45" s="16" t="s">
+        <v>32</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="D45" s="21" t="s">
-        <v>27</v>
+      <c r="B45" s="20"/>
+      <c r="D45" s="16" t="s">
+        <v>33</v>
       </c>
-      <c r="E45" s="22"/>
+      <c r="E45" s="20"/>
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1">
@@ -8515,136 +8555,136 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A47" s="15"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="12"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="15"/>
+      <c r="D47" s="13"/>
       <c r="E47" s="12"/>
       <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
       <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A51" s="15"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="12"/>
-      <c r="D51" s="15"/>
+      <c r="D51" s="13"/>
       <c r="E51" s="12"/>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A55" s="16"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D55" s="16"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="9"/>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A56" s="17"/>
+      <c r="A56" s="23"/>
       <c r="B56" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D56" s="17"/>
+      <c r="D56" s="23"/>
       <c r="E56" s="9"/>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A57" s="17"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D57" s="17"/>
+      <c r="D57" s="23"/>
       <c r="E57" s="9"/>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A58" s="17"/>
+      <c r="A58" s="23"/>
       <c r="B58" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D58" s="17"/>
+      <c r="D58" s="23"/>
       <c r="E58" s="9"/>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A59" s="18"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="D59" s="18"/>
+      <c r="D59" s="24"/>
       <c r="E59" s="10"/>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A60" s="15"/>
+      <c r="A60" s="13"/>
       <c r="B60" s="12"/>
-      <c r="D60" s="15"/>
+      <c r="D60" s="13"/>
       <c r="E60" s="12"/>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1">

</xml_diff>